<commit_message>
lunes en la noche junio 2017
</commit_message>
<xml_diff>
--- a/PowerBI/BD Dash/BD_PDN.xlsx
+++ b/PowerBI/BD Dash/BD_PDN.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelleyton/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.leyton\MiDjango_\tutorial_P3_4\PowerBI\BD Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="460" windowWidth="27380" windowHeight="28060" activeTab="2"/>
+    <workbookView xWindow="15480" yWindow="465" windowWidth="27375" windowHeight="28065" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="237">
   <si>
     <t>Sacos de Cemento</t>
   </si>
@@ -530,9 +530,6 @@
     <t>Completar lunes 15may17</t>
   </si>
   <si>
-    <t>PDN-11</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Supervisión Sondajes Hidrogeológicos</t>
   </si>
   <si>
@@ -575,9 +572,6 @@
     <t>Relincho_Stockpile_Cost_Estimate_</t>
   </si>
   <si>
-    <t>PDN-02</t>
-  </si>
-  <si>
     <t>Geotechnical Logging / PLI Testing Training (Pineda Visit)</t>
   </si>
   <si>
@@ -623,9 +617,6 @@
     <t>ODC n°3</t>
   </si>
   <si>
-    <t>PDN-03</t>
-  </si>
-  <si>
     <t>supplementary tasks by defined shutdowns tasksestimated</t>
   </si>
   <si>
@@ -726,20 +717,53 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>PDN-001</t>
+  </si>
+  <si>
+    <t>PDN-002</t>
+  </si>
+  <si>
+    <t>PDN-003</t>
+  </si>
+  <si>
+    <t>PDN-004</t>
+  </si>
+  <si>
+    <t>PDN-005</t>
+  </si>
+  <si>
+    <t>PDN-006</t>
+  </si>
+  <si>
+    <t>PDN-007</t>
+  </si>
+  <si>
+    <t>PDN-008</t>
+  </si>
+  <si>
+    <t>PDN-009</t>
+  </si>
+  <si>
+    <t>PDN-010</t>
+  </si>
+  <si>
+    <t>PDN-011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -1238,10 +1262,10 @@
   </borders>
   <cellStyleXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1269,10 +1293,10 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1366,7 +1390,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1387,10 +1411,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1399,7 +1423,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1435,7 +1459,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1465,7 +1489,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1474,7 +1498,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1505,7 +1529,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1958,7 +1982,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:R124"/>
@@ -1967,26 +1991,26 @@
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="2"/>
+    <col min="15" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:18" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="42" t="s">
         <v>8</v>
       </c>
@@ -2027,7 +2051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:18" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32"/>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -2042,7 +2066,7 @@
       <c r="M3" s="40"/>
       <c r="N3" s="41"/>
     </row>
-    <row r="4" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>35</v>
       </c>
@@ -2081,7 +2105,7 @@
       </c>
       <c r="N4" s="19"/>
     </row>
-    <row r="5" spans="2:18" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="32"/>
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
@@ -2096,7 +2120,7 @@
       <c r="M5" s="40"/>
       <c r="N5" s="41"/>
     </row>
-    <row r="6" spans="2:18" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>23</v>
       </c>
@@ -2141,7 +2165,7 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
     </row>
-    <row r="7" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
@@ -2176,7 +2200,7 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>23</v>
       </c>
@@ -2211,7 +2235,7 @@
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>23</v>
       </c>
@@ -2246,7 +2270,7 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="2:18" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
@@ -2281,7 +2305,7 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
     </row>
-    <row r="11" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
@@ -2312,7 +2336,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2331,7 +2355,7 @@
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
     </row>
-    <row r="13" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
@@ -2354,7 +2378,7 @@
       <c r="M13" s="30"/>
       <c r="N13" s="31"/>
     </row>
-    <row r="14" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2377,7 +2401,7 @@
       <c r="M14" s="30"/>
       <c r="N14" s="31"/>
     </row>
-    <row r="15" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
@@ -2400,7 +2424,7 @@
       <c r="M15" s="30"/>
       <c r="N15" s="31"/>
     </row>
-    <row r="16" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
@@ -2423,7 +2447,7 @@
       <c r="M16" s="30"/>
       <c r="N16" s="31"/>
     </row>
-    <row r="17" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="32"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
@@ -2438,7 +2462,7 @@
       <c r="M17" s="40"/>
       <c r="N17" s="41"/>
     </row>
-    <row r="18" spans="2:14" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>19</v>
       </c>
@@ -2467,7 +2491,7 @@
       <c r="M18" s="15"/>
       <c r="N18" s="19"/>
     </row>
-    <row r="19" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
@@ -2482,7 +2506,7 @@
       <c r="M19" s="40"/>
       <c r="N19" s="41"/>
     </row>
-    <row r="20" spans="2:14" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
         <v>44</v>
       </c>
@@ -2523,7 +2547,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
@@ -2538,7 +2562,7 @@
       <c r="M21" s="40"/>
       <c r="N21" s="41"/>
     </row>
-    <row r="22" spans="2:14" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" s="3" customFormat="1" ht="84" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>17</v>
       </c>
@@ -2577,7 +2601,7 @@
       </c>
       <c r="N22" s="19"/>
     </row>
-    <row r="23" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
@@ -2606,7 +2630,7 @@
       </c>
       <c r="N23" s="19"/>
     </row>
-    <row r="24" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>17</v>
       </c>
@@ -2635,7 +2659,7 @@
       </c>
       <c r="N24" s="19"/>
     </row>
-    <row r="25" spans="2:14" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>17</v>
       </c>
@@ -2664,7 +2688,7 @@
       </c>
       <c r="N25" s="19"/>
     </row>
-    <row r="26" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>17</v>
       </c>
@@ -2693,7 +2717,7 @@
       </c>
       <c r="N26" s="19"/>
     </row>
-    <row r="27" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>17</v>
       </c>
@@ -2722,7 +2746,7 @@
       </c>
       <c r="N27" s="19"/>
     </row>
-    <row r="28" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
@@ -2737,7 +2761,7 @@
       <c r="M28" s="40"/>
       <c r="N28" s="41"/>
     </row>
-    <row r="29" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>10</v>
       </c>
@@ -2766,7 +2790,7 @@
       </c>
       <c r="N29" s="19"/>
     </row>
-    <row r="30" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>10</v>
       </c>
@@ -2795,7 +2819,7 @@
       </c>
       <c r="N30" s="19"/>
     </row>
-    <row r="31" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>10</v>
       </c>
@@ -2824,7 +2848,7 @@
       </c>
       <c r="N31" s="19"/>
     </row>
-    <row r="32" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>10</v>
       </c>
@@ -2853,7 +2877,7 @@
       </c>
       <c r="N32" s="19"/>
     </row>
-    <row r="33" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>10</v>
       </c>
@@ -2882,7 +2906,7 @@
       </c>
       <c r="N33" s="20"/>
     </row>
-    <row r="34" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>10</v>
       </c>
@@ -2911,7 +2935,7 @@
       </c>
       <c r="N34" s="19"/>
     </row>
-    <row r="35" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>10</v>
       </c>
@@ -2940,7 +2964,7 @@
       </c>
       <c r="N35" s="20"/>
     </row>
-    <row r="36" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>10</v>
       </c>
@@ -2969,7 +2993,7 @@
       </c>
       <c r="N36" s="19"/>
     </row>
-    <row r="37" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
@@ -2984,7 +3008,7 @@
       <c r="M37" s="40"/>
       <c r="N37" s="41"/>
     </row>
-    <row r="38" spans="2:14" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:14" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="B38" s="23" t="s">
         <v>21</v>
       </c>
@@ -3019,7 +3043,7 @@
       </c>
       <c r="N38" s="19"/>
     </row>
-    <row r="39" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="32"/>
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
@@ -3034,7 +3058,7 @@
       <c r="M39" s="40"/>
       <c r="N39" s="41"/>
     </row>
-    <row r="40" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="B40" s="23" t="s">
         <v>32</v>
       </c>
@@ -3075,7 +3099,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>32</v>
       </c>
@@ -3106,7 +3130,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>32</v>
       </c>
@@ -3137,7 +3161,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>32</v>
       </c>
@@ -3168,7 +3192,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>32</v>
       </c>
@@ -3199,7 +3223,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>32</v>
       </c>
@@ -3230,7 +3254,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>32</v>
       </c>
@@ -3261,7 +3285,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
         <v>32</v>
       </c>
@@ -3292,7 +3316,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>32</v>
       </c>
@@ -3323,7 +3347,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
         <v>32</v>
       </c>
@@ -3354,7 +3378,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>32</v>
       </c>
@@ -3385,7 +3409,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>32</v>
       </c>
@@ -3416,7 +3440,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
         <v>32</v>
       </c>
@@ -3447,7 +3471,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
         <v>32</v>
       </c>
@@ -3478,7 +3502,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>32</v>
       </c>
@@ -3509,7 +3533,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>32</v>
       </c>
@@ -3540,7 +3564,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>32</v>
       </c>
@@ -3571,7 +3595,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
         <v>32</v>
       </c>
@@ -3602,7 +3626,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>32</v>
       </c>
@@ -3633,7 +3657,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="59" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
         <v>32</v>
       </c>
@@ -3664,7 +3688,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
         <v>32</v>
       </c>
@@ -3695,7 +3719,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>32</v>
       </c>
@@ -3726,7 +3750,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="6" t="s">
         <v>32</v>
       </c>
@@ -3757,7 +3781,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -3772,7 +3796,7 @@
       <c r="M63" s="15"/>
       <c r="N63" s="19"/>
     </row>
-    <row r="64" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
         <v>32</v>
       </c>
@@ -3801,7 +3825,7 @@
       </c>
       <c r="N64" s="19"/>
     </row>
-    <row r="65" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
         <v>32</v>
       </c>
@@ -3830,7 +3854,7 @@
       </c>
       <c r="N65" s="19"/>
     </row>
-    <row r="66" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
         <v>32</v>
       </c>
@@ -3859,7 +3883,7 @@
       </c>
       <c r="N66" s="19"/>
     </row>
-    <row r="67" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
         <v>32</v>
       </c>
@@ -3888,7 +3912,7 @@
       </c>
       <c r="N67" s="19"/>
     </row>
-    <row r="68" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="6" t="s">
         <v>32</v>
       </c>
@@ -3917,7 +3941,7 @@
       </c>
       <c r="N68" s="19"/>
     </row>
-    <row r="69" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
         <v>32</v>
       </c>
@@ -3946,7 +3970,7 @@
       </c>
       <c r="N69" s="19"/>
     </row>
-    <row r="70" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="6" t="s">
         <v>32</v>
       </c>
@@ -3975,7 +3999,7 @@
       </c>
       <c r="N70" s="19"/>
     </row>
-    <row r="71" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="6" t="s">
         <v>32</v>
       </c>
@@ -4004,7 +4028,7 @@
       </c>
       <c r="N71" s="19"/>
     </row>
-    <row r="72" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="6" t="s">
         <v>32</v>
       </c>
@@ -4033,7 +4057,7 @@
       </c>
       <c r="N72" s="19"/>
     </row>
-    <row r="73" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
         <v>32</v>
       </c>
@@ -4052,7 +4076,7 @@
       <c r="M73" s="17"/>
       <c r="N73" s="19"/>
     </row>
-    <row r="74" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="6" t="s">
         <v>32</v>
       </c>
@@ -4081,7 +4105,7 @@
       </c>
       <c r="N74" s="19"/>
     </row>
-    <row r="75" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
         <v>32</v>
       </c>
@@ -4110,7 +4134,7 @@
       </c>
       <c r="N75" s="19"/>
     </row>
-    <row r="76" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="6" t="s">
         <v>32</v>
       </c>
@@ -4139,7 +4163,7 @@
       </c>
       <c r="N76" s="19"/>
     </row>
-    <row r="77" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="6" t="s">
         <v>32</v>
       </c>
@@ -4168,7 +4192,7 @@
       </c>
       <c r="N77" s="19"/>
     </row>
-    <row r="78" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="6" t="s">
         <v>32</v>
       </c>
@@ -4197,7 +4221,7 @@
       </c>
       <c r="N78" s="19"/>
     </row>
-    <row r="79" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="s">
         <v>32</v>
       </c>
@@ -4226,7 +4250,7 @@
       </c>
       <c r="N79" s="19"/>
     </row>
-    <row r="80" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -4241,7 +4265,7 @@
       <c r="M80" s="15"/>
       <c r="N80" s="19"/>
     </row>
-    <row r="81" spans="2:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:14" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="B81" s="23" t="s">
         <v>32</v>
       </c>
@@ -4282,7 +4306,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="82" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="s">
         <v>32</v>
       </c>
@@ -4313,7 +4337,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="83" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
         <v>32</v>
       </c>
@@ -4344,7 +4368,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="84" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
         <v>32</v>
       </c>
@@ -4375,7 +4399,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="85" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="6" t="s">
         <v>32</v>
       </c>
@@ -4406,7 +4430,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="86" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="6" t="s">
         <v>32</v>
       </c>
@@ -4437,7 +4461,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="87" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="6" t="s">
         <v>32</v>
       </c>
@@ -4468,7 +4492,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="88" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="s">
         <v>32</v>
       </c>
@@ -4499,7 +4523,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="6" t="s">
         <v>32</v>
       </c>
@@ -4530,7 +4554,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="90" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="6" t="s">
         <v>32</v>
       </c>
@@ -4561,7 +4585,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
         <v>32</v>
       </c>
@@ -4592,7 +4616,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
         <v>32</v>
       </c>
@@ -4623,7 +4647,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="93" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="6" t="s">
         <v>32</v>
       </c>
@@ -4654,7 +4678,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="94" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="6" t="s">
         <v>32</v>
       </c>
@@ -4685,7 +4709,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="95" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="6" t="s">
         <v>32</v>
       </c>
@@ -4716,7 +4740,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="6" t="s">
         <v>32</v>
       </c>
@@ -4747,7 +4771,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="97" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="6" t="s">
         <v>32</v>
       </c>
@@ -4778,7 +4802,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="98" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="6" t="s">
         <v>32</v>
       </c>
@@ -4809,7 +4833,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="99" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="6" t="s">
         <v>32</v>
       </c>
@@ -4840,7 +4864,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="100" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="6" t="s">
         <v>32</v>
       </c>
@@ -4871,7 +4895,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="101" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
         <v>32</v>
       </c>
@@ -4902,7 +4926,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="102" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="6" t="s">
         <v>32</v>
       </c>
@@ -4933,7 +4957,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="103" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
         <v>32</v>
       </c>
@@ -4964,7 +4988,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="104" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
@@ -4979,7 +5003,7 @@
       <c r="M104" s="15"/>
       <c r="N104" s="19"/>
     </row>
-    <row r="105" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="6" t="s">
         <v>32</v>
       </c>
@@ -5008,7 +5032,7 @@
       </c>
       <c r="N105" s="19"/>
     </row>
-    <row r="106" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="6" t="s">
         <v>32</v>
       </c>
@@ -5037,7 +5061,7 @@
       </c>
       <c r="N106" s="19"/>
     </row>
-    <row r="107" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="6" t="s">
         <v>32</v>
       </c>
@@ -5066,7 +5090,7 @@
       </c>
       <c r="N107" s="19"/>
     </row>
-    <row r="108" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="6" t="s">
         <v>32</v>
       </c>
@@ -5095,7 +5119,7 @@
       </c>
       <c r="N108" s="19"/>
     </row>
-    <row r="109" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="6" t="s">
         <v>32</v>
       </c>
@@ -5124,7 +5148,7 @@
       </c>
       <c r="N109" s="19"/>
     </row>
-    <row r="110" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="6" t="s">
         <v>32</v>
       </c>
@@ -5153,7 +5177,7 @@
       </c>
       <c r="N110" s="19"/>
     </row>
-    <row r="111" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="6" t="s">
         <v>32</v>
       </c>
@@ -5182,7 +5206,7 @@
       </c>
       <c r="N111" s="19"/>
     </row>
-    <row r="112" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B112" s="6" t="s">
         <v>32</v>
       </c>
@@ -5211,7 +5235,7 @@
       </c>
       <c r="N112" s="19"/>
     </row>
-    <row r="113" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="6" t="s">
         <v>32</v>
       </c>
@@ -5240,7 +5264,7 @@
       </c>
       <c r="N113" s="19"/>
     </row>
-    <row r="114" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="6" t="s">
         <v>32</v>
       </c>
@@ -5259,7 +5283,7 @@
       <c r="M114" s="15"/>
       <c r="N114" s="19"/>
     </row>
-    <row r="115" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="6" t="s">
         <v>32</v>
       </c>
@@ -5288,7 +5312,7 @@
       </c>
       <c r="N115" s="19"/>
     </row>
-    <row r="116" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="6" t="s">
         <v>32</v>
       </c>
@@ -5317,7 +5341,7 @@
       </c>
       <c r="N116" s="19"/>
     </row>
-    <row r="117" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="6" t="s">
         <v>32</v>
       </c>
@@ -5346,7 +5370,7 @@
       </c>
       <c r="N117" s="19"/>
     </row>
-    <row r="118" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="6" t="s">
         <v>32</v>
       </c>
@@ -5375,7 +5399,7 @@
       </c>
       <c r="N118" s="19"/>
     </row>
-    <row r="119" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="6" t="s">
         <v>32</v>
       </c>
@@ -5404,7 +5428,7 @@
       </c>
       <c r="N119" s="19"/>
     </row>
-    <row r="120" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="6" t="s">
         <v>32</v>
       </c>
@@ -5433,7 +5457,7 @@
       </c>
       <c r="N120" s="19"/>
     </row>
-    <row r="121" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:14" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="32"/>
       <c r="C121" s="33"/>
       <c r="D121" s="33"/>
@@ -5448,7 +5472,7 @@
       <c r="M121" s="40"/>
       <c r="N121" s="41"/>
     </row>
-    <row r="122" spans="2:14" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:14" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="B122" s="23" t="s">
         <v>30</v>
       </c>
@@ -5477,14 +5501,14 @@
       <c r="M122" s="15"/>
       <c r="N122" s="19"/>
     </row>
-    <row r="123" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="J123" s="2"/>
     </row>
-    <row r="124" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="124" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
@@ -5505,7 +5529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5513,28 +5537,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="47" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="21" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="18.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>8</v>
       </c>
@@ -5554,32 +5578,32 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="C2" s="49">
         <v>6410210</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="C3" s="55">
         <v>3328</v>
@@ -5588,18 +5612,18 @@
         <v>38</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="C4" s="46">
         <v>372.68</v>
@@ -5608,18 +5632,18 @@
         <v>48</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>227</v>
       </c>
       <c r="C5" s="46">
         <v>273.60000000000002</v>
@@ -5628,18 +5652,18 @@
         <v>49</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
       <c r="C6" s="46">
         <v>271.73</v>
@@ -5648,18 +5672,18 @@
         <v>50</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>229</v>
       </c>
       <c r="C7" s="46">
         <v>220495.62</v>
@@ -5668,18 +5692,18 @@
         <v>59</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>230</v>
       </c>
       <c r="C8" s="46">
         <v>1220.93</v>
@@ -5688,13 +5712,13 @@
         <v>51</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -5708,128 +5732,128 @@
         <v>66</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>231</v>
       </c>
       <c r="C10" s="49">
         <v>2000</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>55</v>
+        <v>232</v>
       </c>
       <c r="C11" s="54">
         <v>387.9</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E11" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>56</v>
+        <v>233</v>
       </c>
       <c r="C12" s="49">
         <v>4000</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" s="48" t="s">
         <v>156</v>
       </c>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>57</v>
+        <v>234</v>
       </c>
       <c r="C13" s="49">
         <v>800</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E13" s="48" t="s">
         <v>156</v>
       </c>
       <c r="F13" s="16"/>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>58</v>
+        <v>235</v>
       </c>
       <c r="C14" s="49">
         <v>55000</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E14" s="48" t="s">
         <v>156</v>
       </c>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>163</v>
+        <v>236</v>
       </c>
       <c r="C15" s="49">
         <v>20000</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E15" s="48" t="s">
         <v>156</v>
       </c>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="C16" s="46">
         <v>-295189</v>
@@ -5838,18 +5862,18 @@
         <v>64</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="C17" s="46">
         <v>42079675</v>
@@ -5862,12 +5886,12 @@
       </c>
       <c r="F17" s="19"/>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
+        <v>227</v>
       </c>
       <c r="C18" s="46">
         <v>4357440</v>
@@ -5880,12 +5904,12 @@
       </c>
       <c r="F18" s="19"/>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
       <c r="C19" s="46">
         <v>2068657.9750000001</v>
@@ -5898,12 +5922,12 @@
       </c>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>28</v>
+        <v>229</v>
       </c>
       <c r="C20" s="46">
         <v>1835064</v>
@@ -5916,12 +5940,12 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>29</v>
+        <v>230</v>
       </c>
       <c r="C21" s="46">
         <v>2345160</v>
@@ -5934,12 +5958,12 @@
       </c>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>54</v>
+        <v>231</v>
       </c>
       <c r="C22" s="46">
         <v>3801600</v>
@@ -5952,32 +5976,32 @@
       </c>
       <c r="F22" s="19"/>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C23" s="46">
         <v>62913093.700000003</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C24" s="46">
         <v>1817575</v>
@@ -5990,12 +6014,12 @@
       </c>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C25" s="46">
         <v>21341930</v>
@@ -6008,12 +6032,12 @@
       </c>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C26" s="46">
         <v>4520995</v>
@@ -6026,12 +6050,12 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C27" s="46">
         <v>4140000</v>
@@ -6044,12 +6068,12 @@
       </c>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C28" s="46">
         <v>5084821.5</v>
@@ -6062,12 +6086,12 @@
       </c>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C29" s="46">
         <v>5175000</v>
@@ -6080,12 +6104,12 @@
       </c>
       <c r="F29" s="20"/>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C30" s="46">
         <v>59446213</v>
@@ -6098,247 +6122,247 @@
       </c>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C31" s="46">
         <v>5420</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C32" s="46">
         <v>6129</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C33" s="46">
         <v>25280</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F33" s="19"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C34" s="46">
         <v>10198</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F34" s="19"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C35" s="46">
         <v>35510</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F35" s="19"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C36" s="46">
         <v>27740</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F36" s="19"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C37" s="46">
         <v>12410</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F37" s="19"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C38" s="46">
         <v>10210</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F38" s="19"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A39" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C39" s="46">
         <v>125148</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F39" s="19"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="C40" s="46">
         <v>13008</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F40" s="19"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
       <c r="C41" s="46">
         <v>59900</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F41" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A42" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>194</v>
+        <v>228</v>
       </c>
       <c r="C42" s="46">
         <v>64775</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F42" s="19"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="C43" s="49">
         <v>47859914</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F43" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>82</v>
@@ -6350,15 +6374,15 @@
         <v>105</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>83</v>
@@ -6370,15 +6394,15 @@
         <v>106</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>84</v>
@@ -6390,15 +6414,15 @@
         <v>107</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>85</v>
@@ -6410,15 +6434,15 @@
         <v>108</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>86</v>
@@ -6430,15 +6454,15 @@
         <v>109</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F48" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>87</v>
@@ -6450,15 +6474,15 @@
         <v>110</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F49" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>88</v>
@@ -6470,15 +6494,15 @@
         <v>111</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F50" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>89</v>
@@ -6490,15 +6514,15 @@
         <v>112</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F51" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>90</v>
@@ -6510,15 +6534,15 @@
         <v>113</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F52" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>91</v>
@@ -6530,15 +6554,15 @@
         <v>114</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F53" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>92</v>
@@ -6550,15 +6574,15 @@
         <v>115</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F54" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>93</v>
@@ -6570,15 +6594,15 @@
         <v>116</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F55" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>94</v>
@@ -6590,15 +6614,15 @@
         <v>117</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F56" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>95</v>
@@ -6610,15 +6634,15 @@
         <v>118</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F57" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>96</v>
@@ -6630,15 +6654,15 @@
         <v>119</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F58" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>97</v>
@@ -6650,15 +6674,15 @@
         <v>120</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F59" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>98</v>
@@ -6670,15 +6694,15 @@
         <v>121</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F60" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>99</v>
@@ -6690,15 +6714,15 @@
         <v>122</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F61" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>100</v>
@@ -6710,15 +6734,15 @@
         <v>123</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F62" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>101</v>
@@ -6730,15 +6754,15 @@
         <v>124</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F63" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>102</v>
@@ -6750,15 +6774,15 @@
         <v>125</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F64" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>103</v>
@@ -6770,15 +6794,15 @@
         <v>126</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F65" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>104</v>
@@ -6790,15 +6814,15 @@
         <v>157</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F66" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>130</v>
@@ -6814,9 +6838,9 @@
       </c>
       <c r="F67" s="19"/>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>131</v>
@@ -6828,15 +6852,15 @@
         <v>140</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F68" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>132</v>
@@ -6848,35 +6872,35 @@
         <v>141</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F69" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C70" s="49">
         <v>0</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F70" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>133</v>
@@ -6888,15 +6912,15 @@
         <v>142</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F71" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>134</v>
@@ -6908,15 +6932,15 @@
         <v>143</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F72" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>135</v>
@@ -6928,15 +6952,15 @@
         <v>144</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F73" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>136</v>
@@ -6948,15 +6972,15 @@
         <v>145</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F74" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>137</v>
@@ -6968,15 +6992,15 @@
         <v>158</v>
       </c>
       <c r="E75" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F75" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>138</v>
@@ -6988,33 +7012,33 @@
         <v>159</v>
       </c>
       <c r="E76" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F76" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C77" s="49">
         <v>16000</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F77" s="16"/>
     </row>
-    <row r="78" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>149</v>
@@ -7023,16 +7047,16 @@
         <v>780800</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E78" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F78" s="16"/>
     </row>
-    <row r="79" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>149</v>
@@ -7041,16 +7065,16 @@
         <v>16000</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E79" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F79" s="16"/>
     </row>
-    <row r="80" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>149</v>
@@ -7059,16 +7083,16 @@
         <v>16000</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E80" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F80" s="16"/>
     </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>149</v>
@@ -7077,16 +7101,16 @@
         <v>38400</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E81" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F81" s="16"/>
     </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>149</v>
@@ -7095,16 +7119,16 @@
         <v>64000</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E82" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F82" s="16"/>
     </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>149</v>
@@ -7113,16 +7137,16 @@
         <v>32000</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E83" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F83" s="16"/>
     </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>149</v>
@@ -7131,16 +7155,16 @@
         <v>16000</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E84" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F84" s="16"/>
     </row>
-    <row r="85" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>149</v>
@@ -7149,16 +7173,16 @@
         <v>16000</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E85" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F85" s="16"/>
     </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>149</v>
@@ -7167,16 +7191,16 @@
         <v>0</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E86" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F86" s="16"/>
     </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>149</v>
@@ -7185,16 +7209,16 @@
         <v>0</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E87" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F87" s="16"/>
     </row>
-    <row r="88" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>149</v>
@@ -7203,16 +7227,16 @@
         <v>30000</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E88" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F88" s="16"/>
     </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>149</v>
@@ -7221,16 +7245,16 @@
         <v>0</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E89" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F89" s="16"/>
     </row>
-    <row r="90" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>149</v>
@@ -7239,16 +7263,16 @@
         <v>0</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E90" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F90" s="16"/>
     </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>149</v>
@@ -7257,16 +7281,16 @@
         <v>0</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E91" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F91" s="16"/>
     </row>
-    <row r="92" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>149</v>
@@ -7275,16 +7299,16 @@
         <v>0</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E92" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F92" s="16"/>
     </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>149</v>
@@ -7293,16 +7317,16 @@
         <v>25600</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E93" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F93" s="16"/>
     </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>82</v>
@@ -7314,15 +7338,15 @@
         <v>105</v>
       </c>
       <c r="E94" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F94" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>83</v>
@@ -7334,15 +7358,15 @@
         <v>106</v>
       </c>
       <c r="E95" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F95" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>84</v>
@@ -7354,15 +7378,15 @@
         <v>107</v>
       </c>
       <c r="E96" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F96" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>85</v>
@@ -7374,15 +7398,15 @@
         <v>108</v>
       </c>
       <c r="E97" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F97" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>86</v>
@@ -7394,15 +7418,15 @@
         <v>109</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F98" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>87</v>
@@ -7414,15 +7438,15 @@
         <v>110</v>
       </c>
       <c r="E99" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F99" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>88</v>
@@ -7434,15 +7458,15 @@
         <v>111</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F100" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>89</v>
@@ -7454,15 +7478,15 @@
         <v>112</v>
       </c>
       <c r="E101" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F101" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>90</v>
@@ -7474,15 +7498,15 @@
         <v>113</v>
       </c>
       <c r="E102" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F102" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>91</v>
@@ -7494,15 +7518,15 @@
         <v>114</v>
       </c>
       <c r="E103" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F103" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>92</v>
@@ -7514,15 +7538,15 @@
         <v>115</v>
       </c>
       <c r="E104" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F104" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>93</v>
@@ -7534,15 +7558,15 @@
         <v>116</v>
       </c>
       <c r="E105" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F105" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>94</v>
@@ -7554,15 +7578,15 @@
         <v>117</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F106" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>95</v>
@@ -7574,15 +7598,15 @@
         <v>118</v>
       </c>
       <c r="E107" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F107" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>96</v>
@@ -7594,15 +7618,15 @@
         <v>119</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F108" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="109" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>97</v>
@@ -7614,15 +7638,15 @@
         <v>120</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F109" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>98</v>
@@ -7634,15 +7658,15 @@
         <v>121</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F110" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="111" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>99</v>
@@ -7654,15 +7678,15 @@
         <v>122</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F111" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="112" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>100</v>
@@ -7674,15 +7698,15 @@
         <v>123</v>
       </c>
       <c r="E112" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F112" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="113" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>101</v>
@@ -7694,15 +7718,15 @@
         <v>124</v>
       </c>
       <c r="E113" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F113" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="114" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>102</v>
@@ -7714,15 +7738,15 @@
         <v>125</v>
       </c>
       <c r="E114" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F114" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>103</v>
@@ -7734,15 +7758,15 @@
         <v>126</v>
       </c>
       <c r="E115" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F115" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="116" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>104</v>
@@ -7754,15 +7778,15 @@
         <v>127</v>
       </c>
       <c r="E116" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F116" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="117" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>130</v>
@@ -7778,9 +7802,9 @@
       </c>
       <c r="F117" s="19"/>
     </row>
-    <row r="118" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>131</v>
@@ -7792,15 +7816,15 @@
         <v>140</v>
       </c>
       <c r="E118" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F118" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="119" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>132</v>
@@ -7812,15 +7836,15 @@
         <v>141</v>
       </c>
       <c r="E119" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F119" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="120" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>133</v>
@@ -7832,15 +7856,15 @@
         <v>142</v>
       </c>
       <c r="E120" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F120" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="121" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>134</v>
@@ -7852,15 +7876,15 @@
         <v>143</v>
       </c>
       <c r="E121" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F121" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="122" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>135</v>
@@ -7872,15 +7896,15 @@
         <v>144</v>
       </c>
       <c r="E122" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F122" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="123" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>136</v>
@@ -7892,15 +7916,15 @@
         <v>145</v>
       </c>
       <c r="E123" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F123" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="124" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>137</v>
@@ -7912,15 +7936,15 @@
         <v>146</v>
       </c>
       <c r="E124" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F124" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="125" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>138</v>
@@ -7932,69 +7956,69 @@
         <v>147</v>
       </c>
       <c r="E125" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F125" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="126" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B126" s="44" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C126" s="46">
         <v>27000000</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E126" s="15" t="s">
         <v>156</v>
       </c>
       <c r="F126" s="19"/>
     </row>
-    <row r="127" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B127" s="44" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C127" s="46">
         <v>12967005</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E127" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F127" s="19"/>
     </row>
-    <row r="128" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B128" s="44" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C128" s="46">
         <v>509990.00000000006</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E128" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F128" s="19"/>
     </row>
-    <row r="129" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B129" s="44" t="s">
         <v>149</v>
@@ -8003,16 +8027,16 @@
         <v>259200000</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E129" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F129" s="19"/>
     </row>
-    <row r="130" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B130" s="44" t="s">
         <v>149</v>
@@ -8021,16 +8045,16 @@
         <v>18000000</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E130" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F130" s="19"/>
     </row>
-    <row r="131" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B131" s="44" t="s">
         <v>149</v>
@@ -8039,16 +8063,16 @@
         <v>18000000</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E131" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F131" s="19"/>
     </row>
-    <row r="132" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B132" s="44" t="s">
         <v>149</v>
@@ -8057,16 +8081,16 @@
         <v>3600000</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E132" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F132" s="19"/>
     </row>
-    <row r="133" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B133" s="44" t="s">
         <v>149</v>
@@ -8075,16 +8099,16 @@
         <v>7200000</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E133" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F133" s="19"/>
     </row>
-    <row r="134" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B134" s="44" t="s">
         <v>149</v>
@@ -8093,16 +8117,16 @@
         <v>14400000</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E134" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F134" s="19"/>
     </row>
-    <row r="135" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B135" s="44" t="s">
         <v>149</v>
@@ -8111,16 +8135,16 @@
         <v>14400000</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E135" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F135" s="19"/>
     </row>
-    <row r="136" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B136" s="44" t="s">
         <v>149</v>
@@ -8129,16 +8153,16 @@
         <v>14400000</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E136" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F136" s="19"/>
     </row>
-    <row r="137" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B137" s="44" t="s">
         <v>149</v>
@@ -8147,16 +8171,16 @@
         <v>3600000</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E137" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F137" s="19"/>
     </row>
-    <row r="138" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B138" s="44" t="s">
         <v>149</v>
@@ -8165,16 +8189,16 @@
         <v>3600000</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E138" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F138" s="19"/>
     </row>
-    <row r="139" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B139" s="44" t="s">
         <v>149</v>
@@ -8183,16 +8207,16 @@
         <v>14400000</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E139" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F139" s="19"/>
     </row>
-    <row r="140" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B140" s="44" t="s">
         <v>149</v>
@@ -8201,16 +8225,16 @@
         <v>3600000</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E140" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F140" s="19"/>
     </row>
-    <row r="141" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B141" s="44" t="s">
         <v>149</v>
@@ -8219,16 +8243,16 @@
         <v>3600000</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E141" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F141" s="19"/>
     </row>
-    <row r="142" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B142" s="44" t="s">
         <v>149</v>
@@ -8237,16 +8261,16 @@
         <v>14400000</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E142" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F142" s="19"/>
     </row>
-    <row r="143" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B143" s="44" t="s">
         <v>149</v>
@@ -8255,16 +8279,16 @@
         <v>28800000</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E143" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F143" s="19"/>
     </row>
-    <row r="144" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B144" s="44" t="s">
         <v>149</v>
@@ -8273,16 +8297,16 @@
         <v>0</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E144" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F144" s="19"/>
     </row>
-    <row r="145" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="52" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>149</v>
@@ -8291,16 +8315,16 @@
         <v>17500000</v>
       </c>
       <c r="D145" s="53" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E145" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F145" s="19"/>
     </row>
-    <row r="146" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="52" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>149</v>
@@ -8309,16 +8333,16 @@
         <v>17500000</v>
       </c>
       <c r="D146" s="53" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E146" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F146" s="19"/>
     </row>
-    <row r="147" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="52" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>149</v>
@@ -8327,16 +8351,16 @@
         <v>75601466</v>
       </c>
       <c r="D147" s="53" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E147" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F147" s="19"/>
     </row>
-    <row r="148" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="52" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>149</v>
@@ -8345,16 +8369,16 @@
         <v>14000000</v>
       </c>
       <c r="D148" s="53" t="s">
+        <v>201</v>
+      </c>
+      <c r="E148" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F148" s="19"/>
+    </row>
+    <row r="149" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="52" t="s">
         <v>204</v>
-      </c>
-      <c r="E148" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="F148" s="19"/>
-    </row>
-    <row r="149" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="52" t="s">
-        <v>207</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>149</v>
@@ -8363,16 +8387,16 @@
         <v>0</v>
       </c>
       <c r="D149" s="53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E149" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F149" s="19"/>
     </row>
-    <row r="150" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="52" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>149</v>
@@ -8381,16 +8405,16 @@
         <v>14000000</v>
       </c>
       <c r="D150" s="53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E150" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F150" s="19"/>
     </row>
-    <row r="151" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="52" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>149</v>
@@ -8399,16 +8423,16 @@
         <v>58692600</v>
       </c>
       <c r="D151" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="E151" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F151" s="19"/>
+    </row>
+    <row r="152" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="52" t="s">
         <v>208</v>
-      </c>
-      <c r="E151" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="F151" s="19"/>
-    </row>
-    <row r="152" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="52" t="s">
-        <v>211</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>149</v>
@@ -8417,16 +8441,16 @@
         <v>0</v>
       </c>
       <c r="D152" s="53" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E152" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F152" s="19"/>
     </row>
-    <row r="153" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="52" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>149</v>
@@ -8435,16 +8459,16 @@
         <v>0</v>
       </c>
       <c r="D153" s="53" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E153" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F153" s="19"/>
     </row>
-    <row r="154" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>94</v>
@@ -8456,15 +8480,15 @@
         <v>117</v>
       </c>
       <c r="E154" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F154" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="155" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B155" s="4" t="s">
         <v>149</v>
@@ -8473,16 +8497,16 @@
         <v>230713371</v>
       </c>
       <c r="D155" s="53" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E155" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F155" s="19"/>
     </row>
-    <row r="156" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B156" s="4" t="s">
         <v>149</v>
@@ -8491,16 +8515,16 @@
         <v>41000000</v>
       </c>
       <c r="D156" s="53" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E156" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F156" s="19"/>
     </row>
-    <row r="157" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>149</v>
@@ -8509,16 +8533,16 @@
         <v>0</v>
       </c>
       <c r="D157" s="53" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E157" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F157" s="19"/>
     </row>
-    <row r="158" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B158" s="4" t="s">
         <v>149</v>
@@ -8527,16 +8551,16 @@
         <v>20500000</v>
       </c>
       <c r="D158" s="53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E158" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F158" s="19"/>
     </row>
-    <row r="159" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>149</v>
@@ -8545,16 +8569,16 @@
         <v>44669791</v>
       </c>
       <c r="D159" s="53" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E159" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F159" s="19"/>
     </row>
-    <row r="160" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>149</v>
@@ -8563,16 +8587,16 @@
         <v>48025753</v>
       </c>
       <c r="D160" s="53" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E160" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F160" s="19"/>
     </row>
-    <row r="161" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>149</v>
@@ -8581,16 +8605,16 @@
         <v>0</v>
       </c>
       <c r="D161" s="53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E161" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F161" s="19"/>
     </row>
-    <row r="162" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="52" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B162" s="4" t="s">
         <v>131</v>
@@ -8602,13 +8626,13 @@
         <v>140</v>
       </c>
       <c r="E162" s="56" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F162" s="19"/>
     </row>
-    <row r="163" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="52" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B163" s="4" t="s">
         <v>136</v>
@@ -8620,13 +8644,13 @@
         <v>145</v>
       </c>
       <c r="E163" s="56" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F163" s="19"/>
     </row>
-    <row r="164" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="52" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>149</v>
@@ -8635,16 +8659,16 @@
         <v>13000000</v>
       </c>
       <c r="D164" s="53" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E164" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F164" s="19"/>
     </row>
-    <row r="165" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="52" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>149</v>
@@ -8653,16 +8677,16 @@
         <v>13000000</v>
       </c>
       <c r="D165" s="53" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E165" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F165" s="19"/>
     </row>
-    <row r="166" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="52" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>149</v>
@@ -8671,16 +8695,16 @@
         <v>13000000</v>
       </c>
       <c r="D166" s="53" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E166" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F166" s="19"/>
     </row>
-    <row r="167" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="52" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>149</v>
@@ -8689,16 +8713,16 @@
         <v>0</v>
       </c>
       <c r="D167" s="53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E167" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F167" s="19"/>
     </row>
-    <row r="168" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="52" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B168" s="4" t="s">
         <v>149</v>
@@ -8707,16 +8731,16 @@
         <v>13000000</v>
       </c>
       <c r="D168" s="53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E168" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F168" s="19"/>
     </row>
-    <row r="169" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="52" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B169" s="4" t="s">
         <v>96</v>
@@ -8728,13 +8752,13 @@
         <v>119</v>
       </c>
       <c r="E169" s="56" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F169" s="19"/>
     </row>
-    <row r="170" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="52" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>149</v>
@@ -8743,16 +8767,16 @@
         <v>8000000</v>
       </c>
       <c r="D170" s="53" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E170" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F170" s="19"/>
     </row>
-    <row r="171" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171" s="52" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>149</v>
@@ -8761,16 +8785,16 @@
         <v>38400000</v>
       </c>
       <c r="D171" s="53" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E171" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F171" s="19"/>
     </row>
-    <row r="172" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="52" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B172" s="4" t="s">
         <v>149</v>
@@ -8779,16 +8803,16 @@
         <v>64000000</v>
       </c>
       <c r="D172" s="53" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E172" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F172" s="19"/>
     </row>
-    <row r="173" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="52" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B173" s="4" t="s">
         <v>149</v>
@@ -8797,16 +8821,16 @@
         <v>0</v>
       </c>
       <c r="D173" s="53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E173" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F173" s="19"/>
     </row>
-    <row r="174" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="52" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B174" s="4" t="s">
         <v>149</v>
@@ -8815,34 +8839,34 @@
         <v>16000000</v>
       </c>
       <c r="D174" s="53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E174" s="17" t="s">
         <v>156</v>
       </c>
       <c r="F174" s="19"/>
     </row>
-    <row r="175" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="52" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C175" s="49">
         <v>45058</v>
       </c>
       <c r="D175" s="53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E175" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F175" s="19"/>
     </row>
-    <row r="176" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="52" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B176" s="4" t="s">
         <v>136</v>
@@ -8854,22 +8878,22 @@
         <v>145</v>
       </c>
       <c r="E176" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F176" s="19"/>
     </row>
-    <row r="177" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" s="52" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C177" s="49">
         <v>31645</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E177" s="17" t="s">
         <v>156</v>
@@ -8889,7 +8913,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -8898,7 +8922,7 @@
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>